<commit_message>
elimination of .csv by .xlsx for correct results
</commit_message>
<xml_diff>
--- a/timeseries count/output.xlsx
+++ b/timeseries count/output.xlsx
@@ -379,7 +379,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -387,159 +387,172 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Sales</t>
+        </is>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Region</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B2" s="1" t="inlineStr">
         <is>
-          <t>Country</t>
+          <t>India</t>
         </is>
       </c>
       <c r="C2" s="1" t="inlineStr">
         <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="D2" s="1" t="inlineStr">
-        <is>
-          <t>Sales</t>
-        </is>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>200</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Asia</t>
-        </is>
-      </c>
+      <c r="A3" s="1" t="n"/>
       <c r="B3" s="1" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>200</v>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>120</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n"/>
+      <c r="B4" s="1" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>175</v>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>150</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n"/>
       <c r="B5" s="1" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="C5" s="1" t="inlineStr">
         <is>
-          <t>D</t>
-        </is>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>325</v>
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>130</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="n"/>
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
       <c r="B6" s="1" t="inlineStr">
         <is>
-          <t>Thailand</t>
+          <t>India</t>
         </is>
       </c>
       <c r="C6" s="1" t="inlineStr">
         <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>150</v>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>175</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="1" t="n"/>
+      <c r="B7" s="1" t="inlineStr">
+        <is>
+          <t>Italy</t>
+        </is>
+      </c>
       <c r="C7" s="1" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D7" s="1" t="n">
+          <t>Europe</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="1" t="inlineStr">
+        <is>
+          <t>Thailand</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
         <v>225</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Europe</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="inlineStr">
-        <is>
-          <t>Italy</t>
-        </is>
-      </c>
-      <c r="C8" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>120</v>
-      </c>
-    </row>
     <row r="9">
-      <c r="A9" s="1" t="n"/>
-      <c r="B9" s="1" t="n"/>
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="inlineStr">
+        <is>
+          <t>Japan</t>
+        </is>
+      </c>
       <c r="C9" s="1" t="inlineStr">
         <is>
-          <t>B</t>
-        </is>
-      </c>
-      <c r="D9" s="1" t="n">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n"/>
-      <c r="B10" s="1" t="inlineStr">
-        <is>
-          <t>Turkey</t>
-        </is>
-      </c>
-      <c r="C10" s="1" t="inlineStr">
-        <is>
-          <t>A</t>
-        </is>
-      </c>
-      <c r="D10" s="1" t="n">
-        <v>130</v>
+          <t>Asia</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A8"/>
   </mergeCells>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>